<commit_message>
new confidence provision to human
</commit_message>
<xml_diff>
--- a/diagrams/excelImage.xlsx
+++ b/diagrams/excelImage.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholaswolczynski/Documents/UT Austin/Research Projects/TeamRules/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholaswolczynski/Documents/UT Austin/Research Projects/TeamRules/diagrams/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45DC945-E9C8-314D-A464-A8A80921D18C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61495A2C-E7F3-9D42-AF15-BE12B77BBA8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20160" xr2:uid="{F742A40B-D5B3-E94B-AA0D-7B3E2048553F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="22">
   <si>
     <t>Age</t>
   </si>
@@ -103,6 +103,9 @@
   <si>
     <t>Ground Truth 
 Outcome</t>
+  </si>
+  <si>
+    <t>AI Confidence</t>
   </si>
 </sst>
 </file>
@@ -158,20 +161,39 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -381,19 +403,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AB136185-B2D6-EF47-A673-5F05E56E049E}" name="Table2" displayName="Table2" ref="D2:N12" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{FCE6EBAC-A0FF-BE4B-BFA3-B5990179B083}" name="Patient" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{3443EF4A-EE63-8D42-883B-9309C81FBFD6}" name="Age" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{4FDA0861-86F3-AB41-A822-4BD82CA1EA18}" name="Weight" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{F6A5BE7C-F4BA-5243-BE3A-ED25F406E6DC}" name="…" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{09B233D3-762B-A043-8DB5-7593D089A913}" name="Doc 1 Initial Diagnosis" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{C8E4C6E2-860F-F044-AB05-B80A39348E38}" name="Doc 1 Confidence" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{963493AE-08C3-A64A-986D-1DB682E2D681}" name="AI Recommendation" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{7922F2EB-C59F-BC42-8633-E7942E0A921C}" name="Doc 1 Final Diagnosis" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{A749BD75-0527-0A4F-882D-640A2C860349}" name="Doc 1 Accepted AI _x000a_Recommendation?" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{FD707DBB-A358-F347-A6FC-F3851CD1BCB6}" name="Likelihood Doc 1 _x000a_Will Accept _x000a_Contradicting AI _x000a_Recommendation " dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{639B7E8B-7B86-D946-9408-925CB10AFFF8}" name="Ground Truth _x000a_Outcome" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AB136185-B2D6-EF47-A673-5F05E56E049E}" name="Table2" displayName="Table2" ref="D2:O12" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{FCE6EBAC-A0FF-BE4B-BFA3-B5990179B083}" name="Patient" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{3443EF4A-EE63-8D42-883B-9309C81FBFD6}" name="Age" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{4FDA0861-86F3-AB41-A822-4BD82CA1EA18}" name="Weight" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{F6A5BE7C-F4BA-5243-BE3A-ED25F406E6DC}" name="…" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{09B233D3-762B-A043-8DB5-7593D089A913}" name="Doc 1 Initial Diagnosis" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{C8E4C6E2-860F-F044-AB05-B80A39348E38}" name="Doc 1 Confidence" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{963493AE-08C3-A64A-986D-1DB682E2D681}" name="AI Recommendation" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{E3008F56-2DB4-0F44-AFF9-0EE6CB54AB6D}" name="AI Confidence" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{7922F2EB-C59F-BC42-8633-E7942E0A921C}" name="Doc 1 Final Diagnosis" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{A749BD75-0527-0A4F-882D-640A2C860349}" name="Doc 1 Accepted AI _x000a_Recommendation?" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{FD707DBB-A358-F347-A6FC-F3851CD1BCB6}" name="Likelihood Doc 1 _x000a_Will Accept _x000a_Contradicting AI _x000a_Recommendation " dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{639B7E8B-7B86-D946-9408-925CB10AFFF8}" name="Ground Truth _x000a_Outcome" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -696,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9200CE92-567D-F94F-A73E-5A8B763A58EE}">
-  <dimension ref="C1:N12"/>
+  <dimension ref="C1:O12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="61" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="131" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -709,23 +732,23 @@
     <col min="6" max="6" width="13.33203125" customWidth="1"/>
     <col min="8" max="8" width="19.83203125" customWidth="1"/>
     <col min="9" max="9" width="16.6640625" customWidth="1"/>
-    <col min="10" max="10" width="20.1640625" customWidth="1"/>
-    <col min="11" max="11" width="19.1640625" customWidth="1"/>
-    <col min="12" max="12" width="17.33203125" customWidth="1"/>
-    <col min="13" max="13" width="15.33203125" customWidth="1"/>
-    <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="20.1640625" customWidth="1"/>
+    <col min="12" max="12" width="19.1640625" customWidth="1"/>
+    <col min="13" max="13" width="17.33203125" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" customWidth="1"/>
+    <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:14" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="3:15" ht="24" x14ac:dyDescent="0.3">
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="2"/>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
@@ -736,391 +759,425 @@
         <v>5</v>
       </c>
       <c r="K1" s="2"/>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="2"/>
+      <c r="M1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="3:14" ht="80" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D2" s="4" t="s">
+    <row r="2" spans="3:15" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="G2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D3" s="4">
-        <v>1</v>
-      </c>
-      <c r="E3" s="4">
+    <row r="3" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3">
         <v>37</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>140</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="4" t="s">
+      <c r="G3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="3">
         <v>0.7</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="3">
+        <v>0.94</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="N3" s="4" t="s">
+      <c r="M3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D4" s="4">
+    <row r="4" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="D4" s="3">
         <v>2</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>52</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>182</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="4" t="s">
+      <c r="G4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <v>0.95</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="4" t="b">
+      <c r="M4" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="M4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="N4" s="4" t="s">
+      <c r="N4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D5" s="4">
+    <row r="5" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="D5" s="3">
         <v>3</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>44</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>119</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="4" t="s">
+      <c r="G5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <v>0.6</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="L5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L5" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="N5" s="4" t="s">
+      <c r="M5" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O5" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4" t="s">
+    <row r="6" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="D6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D7" s="4">
+    <row r="7" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="D7" s="3">
         <v>51</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>53</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>105</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H7" s="4" t="s">
+      <c r="G7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="3">
         <v>0.3</v>
       </c>
-      <c r="J7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M7" s="4">
+      <c r="J7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N7" s="3">
         <v>0.9</v>
       </c>
-      <c r="N7" s="4" t="s">
+      <c r="O7" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D8" s="4">
+    <row r="8" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="D8" s="3">
         <v>52</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>23</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>230</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H8" s="4" t="s">
+      <c r="G8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="3">
         <v>0.89</v>
       </c>
-      <c r="J8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M8" s="4">
+      <c r="J8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N8" s="3">
         <v>0.3</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="O8" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="N9" s="4" t="s">
+    <row r="9" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="D9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O9" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D10" s="4">
+    <row r="10" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="D10" s="3">
         <v>201</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>84</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>114</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H10" s="4" t="s">
+      <c r="G10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="3">
         <v>0.95</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="K10" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="L10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L10" s="4" t="b">
+      <c r="M10" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="M10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="N10" s="4" t="s">
+      <c r="N10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O10" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D11" s="4">
+    <row r="11" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="D11" s="3">
         <v>202</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>26</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>240</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H11" s="4" t="s">
+      <c r="G11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="3">
         <v>0.6</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="J11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="K11" s="3">
+        <v>0.86</v>
+      </c>
+      <c r="L11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L11" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="N11" s="4" t="s">
+      <c r="M11" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O11" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D12" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4" t="s">
+    <row r="12" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="D12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>